<commit_message>
Added paper template filling out necessary sections.
</commit_message>
<xml_diff>
--- a/Project Milestones.xlsx
+++ b/Project Milestones.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22275" windowHeight="15525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Big Data  Project Tasks</t>
   </si>
@@ -38,9 +33,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Get zip code -county mapping and write logic to lookup based on report from inpatient data</t>
-  </si>
-  <si>
     <t>Run MapReduce project on HPC with Inpatient Data</t>
   </si>
   <si>
@@ -81,6 +73,12 @@
   </si>
   <si>
     <t>Spring 2014</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Get zip code-county mapping and write logic to lookup based on report from inpatient data</t>
   </si>
 </sst>
 </file>
@@ -403,7 +401,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -411,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="244" zoomScaleNormal="244" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="244" zoomScaleNormal="244" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,15 +422,15 @@
     <col min="3" max="3" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -442,107 +440,115 @@
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3">
         <v>41736</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3">
         <v>41740</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="3">
         <v>41746</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="3">
         <v>41739</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="3">
         <v>41739</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="3">
+        <v>41736</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="C13" s="3">
         <v>41750</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Checked off some milestone items.
</commit_message>
<xml_diff>
--- a/Project Milestones.xlsx
+++ b/Project Milestones.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22275" windowHeight="15525"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="22275" windowHeight="15465"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Big Data  Project Tasks</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Get zip code-county mapping and write logic to lookup based on report from inpatient data</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -122,13 +125,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,8 +420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="244" zoomScaleNormal="244" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="244" zoomScaleNormal="244" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,6 +429,7 @@
     <col min="1" max="1" width="38.7109375" customWidth="1"/>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
     <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -440,7 +450,7 @@
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -454,6 +464,9 @@
       <c r="C4" s="3">
         <v>41736</v>
       </c>
+      <c r="D4" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -532,6 +545,9 @@
       </c>
       <c r="C12" s="3">
         <v>41736</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adds matlab code to find correlations over time for each county.
</commit_message>
<xml_diff>
--- a/Project Milestones.xlsx
+++ b/Project Milestones.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t>Big Data  Project Tasks</t>
   </si>
@@ -66,12 +66,6 @@
     <t>George</t>
   </si>
   <si>
-    <t>Breakdown existing census  employment data by fields and determine relevant metric</t>
-  </si>
-  <si>
-    <t>Chris, Chen, George</t>
-  </si>
-  <si>
     <t>Spring 2014</t>
   </si>
   <si>
@@ -82,6 +76,42 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>Khen, Chris</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Choose functional attributes for regression (Weka/STATA)</t>
+  </si>
+  <si>
+    <t>Update paper with draft of findings (RESULTS)</t>
+  </si>
+  <si>
+    <t>Update paper with draft of future work</t>
+  </si>
+  <si>
+    <t>Update paper with draft of Conclusions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presentation </t>
+  </si>
+  <si>
+    <t>Presentation Slides and draft script</t>
+  </si>
+  <si>
+    <t>Chris, Khen, George</t>
+  </si>
+  <si>
+    <t>Khen</t>
+  </si>
+  <si>
+    <t>!</t>
+  </si>
+  <si>
+    <t>Breakdown existing census employment data by fields and consolidate into combined results</t>
   </si>
 </sst>
 </file>
@@ -105,12 +135,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -125,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -137,6 +173,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -410,7 +449,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -420,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="244" zoomScaleNormal="244" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,7 +476,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -451,21 +490,21 @@
         <v>3</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C4" s="3">
         <v>41736</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -478,117 +517,186 @@
       <c r="C5" s="3">
         <v>41740</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D5" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C6" s="3">
-        <v>41746</v>
+        <v>41739</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="C7" s="3">
+        <v>41746</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C8" s="3">
-        <v>41739</v>
+        <v>41746</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="3">
+        <v>41739</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="3">
+        <v>41736</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C11" s="3">
-        <v>41739</v>
+        <v>41751</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
+      <c r="A12" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C12" s="3">
-        <v>41736</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>20</v>
+        <v>41752</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
       </c>
       <c r="C13" s="3">
-        <v>41750</v>
+        <v>41753</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="3">
+        <v>41757</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="3">
+        <v>41760</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="3">
+        <v>41760</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="3">
+        <v>41760</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="3">
+        <v>41760</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="3">
+        <v>41767</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
     </row>
   </sheetData>

</xml_diff>